<commit_message>
commit 13674 invoice obh payment list export excel
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.Accounting/eFMS.API.Accounting/Resources/Files/OBHPaymentImportTemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.Accounting/eFMS.API.Accounting/Resources/Files/OBHPaymentImportTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Data\BA Project\Gitlab\eFMS\Tempate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intern.lth007\Desktop\eFMS-WebApp\WebAPI\eFMS.API.SystemWeb\eFMS.API.Accounting\eFMS.API.Accounting\Resources\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -118,12 +118,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,25 +409,25 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" customWidth="1"/>
-    <col min="3" max="3" width="16.36328125" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" customWidth="1"/>
-    <col min="6" max="6" width="14.6328125" customWidth="1"/>
-    <col min="7" max="7" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -444,11 +446,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -465,11 +467,11 @@
       </c>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">

</xml_diff>